<commit_message>
Task 4: separated and moved logics to package
</commit_message>
<xml_diff>
--- a/template_sharing.xlsx
+++ b/template_sharing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t xml:space="preserve">Email</t>
   </si>
@@ -31,13 +31,10 @@
     <t xml:space="preserve">dobzhynetskyy.maksym@chnu.edu.ua</t>
   </si>
   <si>
-    <t xml:space="preserve">1bQ_WbbMkfZazvrl1-SFTna14EEjIloau</t>
+    <t xml:space="preserve">1IOkPPGJij5-OfR1qgz_7srZ00Bzciwa3</t>
   </si>
   <si>
     <t xml:space="preserve">maksym.dobzhinetskii@uvik.net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1faj_6G5_4O9zTrPF61chMbrFyldMgfO1</t>
   </si>
 </sst>
 </file>
@@ -47,7 +44,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -69,6 +66,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="HelveticaNeue"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13"/>
@@ -118,7 +121,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -128,6 +131,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -157,7 +164,7 @@
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="55.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="60.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -180,8 +187,8 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>